<commit_message>
Updated a lot of code.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data_new/data/binned_kcp_data.xlsx
+++ b/DATA/collate_cultivar_data_new/data/binned_kcp_data.xlsx
@@ -409,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D366"/>
+  <dimension ref="A1:D367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,7 +440,7 @@
         <v>182</v>
       </c>
       <c r="D2">
-        <v>0.34035488930685</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -454,7 +454,7 @@
         <v>183</v>
       </c>
       <c r="D3">
-        <v>0.3295579599643464</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -468,7 +468,7 @@
         <v>184</v>
       </c>
       <c r="D4">
-        <v>0.319033890452744</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -482,7 +482,7 @@
         <v>185</v>
       </c>
       <c r="D5">
-        <v>0.3087798824534268</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -496,7 +496,7 @@
         <v>186</v>
       </c>
       <c r="D6">
-        <v>0.2987931432470778</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -510,7 +510,7 @@
         <v>187</v>
       </c>
       <c r="D7">
-        <v>0.2890708857920738</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -524,7 +524,7 @@
         <v>188</v>
       </c>
       <c r="D8">
-        <v>0.2796103288028806</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -538,7 +538,7 @@
         <v>189</v>
       </c>
       <c r="D9">
-        <v>0.2704086968284485</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -552,7 +552,7 @@
         <v>190</v>
       </c>
       <c r="D10">
-        <v>0.2614632203306073</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -566,7 +566,7 @@
         <v>191</v>
       </c>
       <c r="D11">
-        <v>0.2527711357624612</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -580,7 +580,7 @@
         <v>192</v>
       </c>
       <c r="D12">
-        <v>0.2443296856467848</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -594,7 +594,7 @@
         <v>193</v>
       </c>
       <c r="D13">
-        <v>0.2361361186544174</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -608,7 +608,7 @@
         <v>194</v>
       </c>
       <c r="D14">
-        <v>0.228187689682659</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -622,7 +622,7 @@
         <v>195</v>
       </c>
       <c r="D15">
-        <v>0.2204816599336649</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -636,7 +636,7 @@
         <v>196</v>
       </c>
       <c r="D16">
-        <v>0.2130152969928414</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -650,7 +650,7 @@
         <v>197</v>
       </c>
       <c r="D17">
-        <v>0.2057858749072405</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -664,7 +664,7 @@
         <v>198</v>
       </c>
       <c r="D18">
-        <v>0.1987906742639556</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -678,7 +678,7 @@
         <v>199</v>
       </c>
       <c r="D19">
-        <v>0.1920269822685164</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -692,7 +692,7 @@
         <v>200</v>
       </c>
       <c r="D20">
-        <v>0.185492092823284</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -706,7 +706,7 @@
         <v>201</v>
       </c>
       <c r="D21">
-        <v>0.1791833066058467</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -720,7 +720,7 @@
         <v>202</v>
       </c>
       <c r="D22">
-        <v>0.1730979311474145</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -734,7 +734,7 @@
         <v>203</v>
       </c>
       <c r="D23">
-        <v>0.1672332809112147</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -748,7 +748,7 @@
         <v>204</v>
       </c>
       <c r="D24">
-        <v>0.161586677370887</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -762,7 +762,7 @@
         <v>205</v>
       </c>
       <c r="D25">
-        <v>0.1561554490888789</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -776,7 +776,7 @@
         <v>206</v>
       </c>
       <c r="D26">
-        <v>0.1509369317948405</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -790,7 +790,7 @@
         <v>207</v>
       </c>
       <c r="D27">
-        <v>0.14592846846402</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -804,7 +804,7 @@
         <v>208</v>
       </c>
       <c r="D28">
-        <v>0.1411274093956589</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -818,7 +818,7 @@
         <v>209</v>
       </c>
       <c r="D29">
-        <v>0.1365311122913873</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -832,7 +832,7 @@
         <v>210</v>
       </c>
       <c r="D30">
-        <v>0.1321369423336188</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -846,7 +846,7 @@
         <v>211</v>
       </c>
       <c r="D31">
-        <v>0.1279422722639457</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -860,7 +860,7 @@
         <v>212</v>
       </c>
       <c r="D32">
-        <v>0.1239444824615349</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -874,7 +874,7 @@
         <v>213</v>
       </c>
       <c r="D33">
-        <v>0.1201409610215221</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -888,7 +888,7 @@
         <v>214</v>
       </c>
       <c r="D34">
-        <v>0.1165291038334077</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -902,7 +902,7 @@
         <v>215</v>
       </c>
       <c r="D35">
-        <v>0.1131063146594518</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -916,7 +916,7 @@
         <v>216</v>
       </c>
       <c r="D36">
-        <v>0.1098700052130696</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -930,7 +930,7 @@
         <v>217</v>
       </c>
       <c r="D37">
-        <v>0.1068175952372259</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -944,7 +944,7 @@
         <v>218</v>
       </c>
       <c r="D38">
-        <v>0.1039465125828315</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -958,7 +958,7 @@
         <v>219</v>
       </c>
       <c r="D39">
-        <v>0.1012541932871373</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -972,7 +972,7 @@
         <v>220</v>
       </c>
       <c r="D40">
-        <v>0.09873808165212991</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -986,7 +986,7 @@
         <v>221</v>
       </c>
       <c r="D41">
-        <v>0.09639563032292725</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1000,7 +1000,7 @@
         <v>222</v>
       </c>
       <c r="D42">
-        <v>0.0942243003661731</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1014,7 +1014,7 @@
         <v>223</v>
       </c>
       <c r="D43">
-        <v>0.09222156134843276</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1028,7 +1028,7 @@
         <v>224</v>
       </c>
       <c r="D44">
-        <v>0.09038489141458805</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1042,7 +1042,7 @@
         <v>225</v>
       </c>
       <c r="D45">
-        <v>0.08871177736623254</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1056,7 +1056,7 @@
         <v>226</v>
       </c>
       <c r="D46">
-        <v>0.08719971474006688</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1070,7 +1070,7 @@
         <v>227</v>
       </c>
       <c r="D47">
-        <v>0.08584620788629393</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1084,7 +1084,7 @@
         <v>228</v>
       </c>
       <c r="D48">
-        <v>0.08464877004701388</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1098,7 +1098,7 @@
         <v>229</v>
       </c>
       <c r="D49">
-        <v>0.08360492343461956</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1112,7 +1112,7 @@
         <v>230</v>
       </c>
       <c r="D50">
-        <v>0.08271219931019158</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1126,7 +1126,7 @@
         <v>231</v>
       </c>
       <c r="D51">
-        <v>0.08196813806189379</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1140,7 +1140,7 @@
         <v>232</v>
       </c>
       <c r="D52">
-        <v>0.08137028928336809</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1154,7 +1154,7 @@
         <v>233</v>
       </c>
       <c r="D53">
-        <v>0.08091621185212977</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1168,7 +1168,7 @@
         <v>234</v>
       </c>
       <c r="D54">
-        <v>0.08060347400796303</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1182,7 +1182,7 @@
         <v>235</v>
       </c>
       <c r="D55">
-        <v>0.0804296534313157</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1196,7 +1196,7 @@
         <v>236</v>
       </c>
       <c r="D56">
-        <v>0.08039233732169476</v>
+        <v>0.07675116001046195</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1210,7 +1210,7 @@
         <v>237</v>
       </c>
       <c r="D57">
-        <v>0.08048912247606155</v>
+        <v>0.07683243373755488</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1224,7 +1224,7 @@
         <v>238</v>
       </c>
       <c r="D58">
-        <v>0.08071761536722677</v>
+        <v>0.07705628580450402</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1238,7 +1238,7 @@
         <v>239</v>
       </c>
       <c r="D59">
-        <v>0.08107543222224589</v>
+        <v>0.07741986488980307</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1252,7 +1252,7 @@
         <v>240</v>
       </c>
       <c r="D60">
-        <v>0.0815601991008143</v>
+        <v>0.07792033887768712</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1266,7 +1266,7 @@
         <v>241</v>
       </c>
       <c r="D61">
-        <v>0.08216955197366244</v>
+        <v>0.078554894858132</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1280,7 +1280,7 @@
         <v>242</v>
       </c>
       <c r="D62">
-        <v>0.08290113680095118</v>
+        <v>0.07932073912685494</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1294,7 +1294,7 @@
         <v>243</v>
       </c>
       <c r="D63">
-        <v>0.08375260961066672</v>
+        <v>0.08021509718531405</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1308,7 +1308,7 @@
         <v>244</v>
       </c>
       <c r="D64">
-        <v>0.0847216365770162</v>
+        <v>0.08123521374070874</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1322,7 +1322,7 @@
         <v>245</v>
       </c>
       <c r="D65">
-        <v>0.0858058940988225</v>
+        <v>0.08237835270597943</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1336,7 +1336,7 @@
         <v>246</v>
       </c>
       <c r="D66">
-        <v>0.08700306887791998</v>
+        <v>0.08364179719980752</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1350,7 +1350,7 @@
         <v>247</v>
       </c>
       <c r="D67">
-        <v>0.08831085799754895</v>
+        <v>0.08502284954661576</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1364,7 +1364,7 @@
         <v>248</v>
       </c>
       <c r="D68">
-        <v>0.08972696900075167</v>
+        <v>0.08651883127656762</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1378,7 +1378,7 @@
         <v>249</v>
       </c>
       <c r="D69">
-        <v>0.09124911996876675</v>
+        <v>0.08812708312556811</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1392,7 +1392,7 @@
         <v>250</v>
       </c>
       <c r="D70">
-        <v>0.09287503959942517</v>
+        <v>0.0898449650352629</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1406,7 +1406,7 @@
         <v>251</v>
       </c>
       <c r="D71">
-        <v>0.09460246728554503</v>
+        <v>0.09166985615303913</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1420,7 +1420,7 @@
         <v>252</v>
       </c>
       <c r="D72">
-        <v>0.09642915319332657</v>
+        <v>0.0935991548320248</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1434,7 +1434,7 @@
         <v>253</v>
       </c>
       <c r="D73">
-        <v>0.098352858340748</v>
+        <v>0.09563027863108903</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1448,7 +1448,7 @@
         <v>254</v>
       </c>
       <c r="D74">
-        <v>0.1003713546759599</v>
+        <v>0.09776066431484204</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1462,7 +1462,7 @@
         <v>255</v>
       </c>
       <c r="D75">
-        <v>0.1024824251556815</v>
+        <v>0.09998776785363533</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1476,7 +1476,7 @@
         <v>256</v>
       </c>
       <c r="D76">
-        <v>0.1046838638235945</v>
+        <v>0.1023090644235612</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1490,7 +1490,7 @@
         <v>257</v>
       </c>
       <c r="D77">
-        <v>0.1069734758887397</v>
+        <v>0.1047220484064533</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1504,7 +1504,7 @@
         <v>258</v>
       </c>
       <c r="D78">
-        <v>0.109349077803911</v>
+        <v>0.1072242333898862</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1518,7 +1518,7 @@
         <v>259</v>
       </c>
       <c r="D79">
-        <v>0.1118084973440517</v>
+        <v>0.1098131521671757</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1532,7 +1532,7 @@
         <v>260</v>
       </c>
       <c r="D80">
-        <v>0.1143495736846488</v>
+        <v>0.1124863567373784</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1546,7 +1546,7 @@
         <v>261</v>
       </c>
       <c r="D81">
-        <v>0.1169701574801286</v>
+        <v>0.1152414183052927</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1560,7 +1560,7 @@
         <v>262</v>
       </c>
       <c r="D82">
-        <v>0.119668110942252</v>
+        <v>0.1180759272814569</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1574,7 +1574,7 @@
         <v>263</v>
       </c>
       <c r="D83">
-        <v>0.1224413079185094</v>
+        <v>0.1209874932821517</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1588,7 +1588,7 @@
         <v>264</v>
       </c>
       <c r="D84">
-        <v>0.1252876339705163</v>
+        <v>0.1239737451293981</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1602,7 +1602,7 @@
         <v>265</v>
       </c>
       <c r="D85">
-        <v>0.1282049864524082</v>
+        <v>0.1270323308509583</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1616,7 +1616,7 @@
         <v>266</v>
       </c>
       <c r="D86">
-        <v>0.1311912745892358</v>
+        <v>0.1301609176803359</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1630,7 +1630,7 @@
         <v>267</v>
       </c>
       <c r="D87">
-        <v>0.1342444195553605</v>
+        <v>0.1333571920567753</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1644,7 +1644,7 @@
         <v>268</v>
       </c>
       <c r="D88">
-        <v>0.1373623545528493</v>
+        <v>0.136618859625262</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1658,7 +1658,7 @@
         <v>269</v>
       </c>
       <c r="D89">
-        <v>0.1405430248898704</v>
+        <v>0.1399436452365227</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1672,7 +1672,7 @@
         <v>270</v>
       </c>
       <c r="D90">
-        <v>0.1437843880590876</v>
+        <v>0.1433292929470251</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1686,7 +1686,7 @@
         <v>271</v>
       </c>
       <c r="D91">
-        <v>0.1470844138160564</v>
+        <v>0.1467735660189783</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1700,7 +1700,7 @@
         <v>272</v>
       </c>
       <c r="D92">
-        <v>0.150441084257619</v>
+        <v>0.1502742469203321</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1714,7 +1714,7 @@
         <v>273</v>
       </c>
       <c r="D93">
-        <v>0.153852393900299</v>
+        <v>0.1538291373247775</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1728,7 +1728,7 @@
         <v>274</v>
       </c>
       <c r="D94">
-        <v>0.1573163497586974</v>
+        <v>0.1574360581117467</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1742,7 +1742,7 @@
         <v>275</v>
       </c>
       <c r="D95">
-        <v>0.1608309714238868</v>
+        <v>0.161092849366413</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1756,7 +1756,7 @@
         <v>276</v>
       </c>
       <c r="D96">
-        <v>0.1643942911418076</v>
+        <v>0.1647973703796908</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1770,7 +1770,7 @@
         <v>277</v>
       </c>
       <c r="D97">
-        <v>0.1680043538916627</v>
+        <v>0.1685474996482354</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1784,7 +1784,7 @@
         <v>278</v>
       </c>
       <c r="D98">
-        <v>0.1716592174643132</v>
+        <v>0.1723411348744431</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1798,7 +1798,7 @@
         <v>279</v>
       </c>
       <c r="D99">
-        <v>0.1753569525406722</v>
+        <v>0.1761761929664518</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1812,7 +1812,7 @@
         <v>280</v>
       </c>
       <c r="D100">
-        <v>0.179095642770102</v>
+        <v>0.1800506100381403</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1826,7 +1826,7 @@
         <v>281</v>
       </c>
       <c r="D101">
-        <v>0.1828733848488078</v>
+        <v>0.1839623414091285</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1840,7 +1840,7 @@
         <v>282</v>
       </c>
       <c r="D102">
-        <v>0.1866882885982336</v>
+        <v>0.1879093616047767</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1854,7 +1854,7 @@
         <v>283</v>
       </c>
       <c r="D103">
-        <v>0.1905384770434571</v>
+        <v>0.1918896643561874</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1868,7 +1868,7 @@
         <v>284</v>
       </c>
       <c r="D104">
-        <v>0.1944220864915854</v>
+        <v>0.1959012626002037</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1882,7 +1882,7 @@
         <v>285</v>
       </c>
       <c r="D105">
-        <v>0.1983372666101496</v>
+        <v>0.1999421884794096</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1896,7 +1896,7 @@
         <v>286</v>
       </c>
       <c r="D106">
-        <v>0.2022821805055003</v>
+        <v>0.2040104933421305</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1910,7 +1910,7 @@
         <v>287</v>
       </c>
       <c r="D107">
-        <v>0.2062550048012025</v>
+        <v>0.2081042477424327</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1924,7 +1924,7 @@
         <v>288</v>
       </c>
       <c r="D108">
-        <v>0.2102539297164315</v>
+        <v>0.2122215414401238</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1938,7 +1938,7 @@
         <v>289</v>
       </c>
       <c r="D109">
-        <v>0.2142771591443677</v>
+        <v>0.216360483400752</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1952,7 +1952,7 @@
         <v>290</v>
       </c>
       <c r="D110">
-        <v>0.2183229107305916</v>
+        <v>0.2205192017956075</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1966,7 +1966,7 @@
         <v>291</v>
       </c>
       <c r="D111">
-        <v>0.2223894159514787</v>
+        <v>0.2246958440017205</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1980,7 +1980,7 @@
         <v>292</v>
       </c>
       <c r="D112">
-        <v>0.2264749201925962</v>
+        <v>0.2288885766018633</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -1994,7 +1994,7 @@
         <v>293</v>
       </c>
       <c r="D113">
-        <v>0.2305776828270971</v>
+        <v>0.2330955853845488</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2008,7 +2008,7 @@
         <v>294</v>
       </c>
       <c r="D114">
-        <v>0.2346959772941143</v>
+        <v>0.2373150753440308</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2022,7 +2022,7 @@
         <v>295</v>
       </c>
       <c r="D115">
-        <v>0.2388280911771583</v>
+        <v>0.2415452706803046</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2036,7 +2036,7 @@
         <v>296</v>
       </c>
       <c r="D116">
-        <v>0.242972326282511</v>
+        <v>0.245784414799106</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2050,7 +2050,7 @@
         <v>297</v>
       </c>
       <c r="D117">
-        <v>0.2471269987176205</v>
+        <v>0.2500307703119131</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2064,7 +2064,7 @@
         <v>298</v>
       </c>
       <c r="D118">
-        <v>0.2512904389694972</v>
+        <v>0.2542826190359438</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2078,7 +2078,7 @@
         <v>299</v>
       </c>
       <c r="D119">
-        <v>0.2554609919831088</v>
+        <v>0.2585382619941577</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2092,7 +2092,7 @@
         <v>300</v>
       </c>
       <c r="D120">
-        <v>0.2596370172397749</v>
+        <v>0.2627960194152557</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2106,7 +2106,7 @@
         <v>301</v>
       </c>
       <c r="D121">
-        <v>0.2638168888355634</v>
+        <v>0.2670542307336791</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2120,7 +2120,7 @@
         <v>302</v>
       </c>
       <c r="D122">
-        <v>0.2679989955596841</v>
+        <v>0.2713112545896107</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2134,7 +2134,7 @@
         <v>303</v>
       </c>
       <c r="D123">
-        <v>0.2721817409728854</v>
+        <v>0.2755654688289744</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2148,7 +2148,7 @@
         <v>304</v>
       </c>
       <c r="D124">
-        <v>0.2763635434858488</v>
+        <v>0.2798152705034354</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>305</v>
       </c>
       <c r="D125">
-        <v>0.2805428364375843</v>
+        <v>0.2840590758703997</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2176,7 +2176,7 @@
         <v>306</v>
       </c>
       <c r="D126">
-        <v>0.2847180681738251</v>
+        <v>0.2882953203930144</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2190,7 +2190,7 @@
         <v>307</v>
       </c>
       <c r="D127">
-        <v>0.2888877021254237</v>
+        <v>0.292522458740168</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2204,7 +2204,7 @@
         <v>308</v>
       </c>
       <c r="D128">
-        <v>0.2930502168867464</v>
+        <v>0.2967389647864895</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2218,7 +2218,7 @@
         <v>309</v>
       </c>
       <c r="D129">
-        <v>0.2972041062940689</v>
+        <v>0.3009433316123497</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2232,7 +2232,7 @@
         <v>310</v>
       </c>
       <c r="D130">
-        <v>0.3013478795039712</v>
+        <v>0.30513407150386</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2246,7 +2246,7 @@
         <v>311</v>
       </c>
       <c r="D131">
-        <v>0.305480061071733</v>
+        <v>0.3093097159528728</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2260,7 +2260,7 @@
         <v>312</v>
       </c>
       <c r="D132">
-        <v>0.3095991910297288</v>
+        <v>0.3134688156569824</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2274,7 +2274,7 @@
         <v>313</v>
       </c>
       <c r="D133">
-        <v>0.3137038249658232</v>
+        <v>0.3176099405195232</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2288,7 +2288,7 @@
         <v>314</v>
       </c>
       <c r="D134">
-        <v>0.3177925341017664</v>
+        <v>0.3217316796495711</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2302,7 +2302,7 @@
         <v>315</v>
       </c>
       <c r="D135">
-        <v>0.3218639053715883</v>
+        <v>0.3258326413619434</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2316,7 +2316,7 @@
         <v>316</v>
       </c>
       <c r="D136">
-        <v>0.3259165414999957</v>
+        <v>0.3299114531771984</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2330,7 +2330,7 @@
         <v>317</v>
       </c>
       <c r="D137">
-        <v>0.3299490610807652</v>
+        <v>0.3339667618216345</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2344,7 +2344,7 @@
         <v>318</v>
       </c>
       <c r="D138">
-        <v>0.3339600986551394</v>
+        <v>0.3379972332272926</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2358,7 +2358,7 @@
         <v>319</v>
       </c>
       <c r="D139">
-        <v>0.3379483047902241</v>
+        <v>0.3420015525319546</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2372,7 +2372,7 @@
         <v>320</v>
       </c>
       <c r="D140">
-        <v>0.3419123461573791</v>
+        <v>0.3459784240791419</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2386,7 +2386,7 @@
         <v>321</v>
       </c>
       <c r="D141">
-        <v>0.3458509056106178</v>
+        <v>0.3499265714181186</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2400,7 +2400,7 @@
         <v>322</v>
       </c>
       <c r="D142">
-        <v>0.3497626822649994</v>
+        <v>0.3538447373038897</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2414,7 +2414,7 @@
         <v>323</v>
       </c>
       <c r="D143">
-        <v>0.3536463915750258</v>
+        <v>0.3577316836972</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2428,7 +2428,7 @@
         <v>324</v>
       </c>
       <c r="D144">
-        <v>0.3575007654130364</v>
+        <v>0.3615861917645378</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2442,7 +2442,7 @@
         <v>325</v>
       </c>
       <c r="D145">
-        <v>0.3613245521476028</v>
+        <v>0.3654070618781299</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2456,7 +2456,7 @@
         <v>326</v>
       </c>
       <c r="D146">
-        <v>0.3651165167219245</v>
+        <v>0.3691931136159461</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2470,7 +2470,7 @@
         <v>327</v>
       </c>
       <c r="D147">
-        <v>0.3688754407322243</v>
+        <v>0.372943185761696</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2484,7 +2484,7 @@
         <v>328</v>
       </c>
       <c r="D148">
-        <v>0.3726001225061422</v>
+        <v>0.3766561363048313</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2498,7 +2498,7 @@
         <v>329</v>
       </c>
       <c r="D149">
-        <v>0.3762893771811329</v>
+        <v>0.3803308424405442</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2512,7 +2512,7 @@
         <v>330</v>
       </c>
       <c r="D150">
-        <v>0.379942036782859</v>
+        <v>0.3839662005697678</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2526,7 +2526,7 @@
         <v>331</v>
       </c>
       <c r="D151">
-        <v>0.3835569503035864</v>
+        <v>0.3875611262991768</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2540,7 +2540,7 @@
         <v>332</v>
       </c>
       <c r="D152">
-        <v>0.3871329837805813</v>
+        <v>0.3911145544411874</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2554,7 +2554,7 @@
         <v>333</v>
       </c>
       <c r="D153">
-        <v>0.3906690203745038</v>
+        <v>0.3946254390139559</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2568,7 +2568,7 @@
         <v>334</v>
       </c>
       <c r="D154">
-        <v>0.394163960447802</v>
+        <v>0.3980927532413803</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2582,7 +2582,7 @@
         <v>335</v>
       </c>
       <c r="D155">
-        <v>0.3976167216431104</v>
+        <v>0.4015154895530988</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2596,7 +2596,7 @@
         <v>336</v>
       </c>
       <c r="D156">
-        <v>0.4010262389616432</v>
+        <v>0.4048926595844924</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2610,7 +2610,7 @@
         <v>337</v>
       </c>
       <c r="D157">
-        <v>0.4043914648415877</v>
+        <v>0.4082232941766816</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2624,7 +2624,7 @@
         <v>338</v>
       </c>
       <c r="D158">
-        <v>0.4077113692365045</v>
+        <v>0.4115064433765288</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2638,7 +2638,7 @@
         <v>339</v>
       </c>
       <c r="D159">
-        <v>0.4109849396937172</v>
+        <v>0.4147411764366374</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2652,7 +2652,7 @@
         <v>340</v>
       </c>
       <c r="D160">
-        <v>0.4142111814327113</v>
+        <v>0.417926581815351</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2666,7 +2666,7 @@
         <v>341</v>
       </c>
       <c r="D161">
-        <v>0.4173891174235275</v>
+        <v>0.4210617671767561</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2680,7 +2680,7 @@
         <v>342</v>
       </c>
       <c r="D162">
-        <v>0.4205177884651586</v>
+        <v>0.4241458593906793</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2694,7 +2694,7 @@
         <v>343</v>
       </c>
       <c r="D163">
-        <v>0.4235962532639423</v>
+        <v>0.4271780045326874</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2708,7 +2708,7 @@
         <v>344</v>
       </c>
       <c r="D164">
-        <v>0.4266235885119596</v>
+        <v>0.4301573678840899</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2722,7 +2722,7 @@
         <v>345</v>
       </c>
       <c r="D165">
-        <v>0.4295988889654264</v>
+        <v>0.4330831339319365</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2736,7 +2736,7 @@
         <v>346</v>
       </c>
       <c r="D166">
-        <v>0.4325212675230917</v>
+        <v>0.4359545063690174</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2750,7 +2750,7 @@
         <v>347</v>
       </c>
       <c r="D167">
-        <v>0.4353898553046313</v>
+        <v>0.4387707080938658</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2764,7 +2764,7 @@
         <v>348</v>
       </c>
       <c r="D168">
-        <v>0.4382038017290432</v>
+        <v>0.4415309812107545</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2778,7 +2778,7 @@
         <v>349</v>
       </c>
       <c r="D169">
-        <v>0.4409622745930428</v>
+        <v>0.4442345870296975</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2792,7 +2792,7 @@
         <v>350</v>
       </c>
       <c r="D170">
-        <v>0.4436644601494596</v>
+        <v>0.4468808060664504</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2806,7 +2806,7 @@
         <v>351</v>
       </c>
       <c r="D171">
-        <v>0.446309563185629</v>
+        <v>0.4494689380425094</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2820,7 +2820,7 @@
         <v>352</v>
       </c>
       <c r="D172">
-        <v>0.4488968071017915</v>
+        <v>0.4519983018851119</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -2834,7 +2834,7 @@
         <v>353</v>
       </c>
       <c r="D173">
-        <v>0.4514254339894842</v>
+        <v>0.4544682357272368</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -2848,7 +2848,7 @@
         <v>354</v>
       </c>
       <c r="D174">
-        <v>0.4538947047099394</v>
+        <v>0.4568780969076044</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -2862,7 +2862,7 @@
         <v>355</v>
       </c>
       <c r="D175">
-        <v>0.456303898972477</v>
+        <v>0.4592272619706742</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -2876,7 +2876,7 @@
         <v>356</v>
       </c>
       <c r="D176">
-        <v>0.4586523154129016</v>
+        <v>0.4615151266666486</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -2890,7 +2890,7 @@
         <v>357</v>
       </c>
       <c r="D177">
-        <v>0.4609392716718966</v>
+        <v>0.4637411059514707</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -2904,7 +2904,7 @@
         <v>358</v>
       </c>
       <c r="D178">
-        <v>0.4631641044734205</v>
+        <v>0.4659046339868246</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -2918,7 +2918,7 @@
         <v>359</v>
       </c>
       <c r="D179">
-        <v>0.4653261697031006</v>
+        <v>0.4680051641401364</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -2932,7 +2932,7 @@
         <v>360</v>
       </c>
       <c r="D180">
-        <v>0.4674248424866297</v>
+        <v>0.4700421689845707</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -2946,7 +2946,7 @@
         <v>361</v>
       </c>
       <c r="D181">
-        <v>0.4694595172681608</v>
+        <v>0.472015140299036</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -2960,7 +2960,7 @@
         <v>362</v>
       </c>
       <c r="D182">
-        <v>0.4714296078887</v>
+        <v>0.4739235890681801</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -2974,7 +2974,7 @@
         <v>363</v>
       </c>
       <c r="D183">
-        <v>0.4733345476645078</v>
+        <v>0.4757670454823931</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -2988,7 +2988,7 @@
         <v>364</v>
       </c>
       <c r="D184">
-        <v>0.4751737894654862</v>
+        <v>0.4775450589378052</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3002,7 +3002,7 @@
         <v>365</v>
       </c>
       <c r="D185">
-        <v>0.4769468057935817</v>
+        <v>0.479257198036289</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
       <c r="D186">
-        <v>0.478653088861174</v>
+        <v>0.4809030505854567</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -3030,7 +3030,7 @@
         <v>2</v>
       </c>
       <c r="D187">
-        <v>0.4802921506694762</v>
+        <v>0.4824822235986623</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -3044,7 +3044,7 @@
         <v>3</v>
       </c>
       <c r="D188">
-        <v>0.4818635230869264</v>
+        <v>0.4839943432950009</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -3058,7 +3058,7 @@
         <v>4</v>
       </c>
       <c r="D189">
-        <v>0.4833667579275849</v>
+        <v>0.4854390550993086</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -3072,7 +3072,7 @@
         <v>5</v>
       </c>
       <c r="D190">
-        <v>0.4848014270295303</v>
+        <v>0.4868160236421625</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -3086,7 +3086,7 @@
         <v>6</v>
       </c>
       <c r="D191">
-        <v>0.4861671223332505</v>
+        <v>0.4881249327598814</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -3100,7 +3100,7 @@
         <v>7</v>
       </c>
       <c r="D192">
-        <v>0.4874634559600431</v>
+        <v>0.4893654854945237</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -3114,7 +3114,7 @@
         <v>8</v>
       </c>
       <c r="D193">
-        <v>0.4886900602904078</v>
+        <v>0.490537404093891</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -3128,7 +3128,7 @@
         <v>9</v>
       </c>
       <c r="D194">
-        <v>0.489846588042441</v>
+        <v>0.4916404300115237</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -3142,7 +3142,7 @@
         <v>10</v>
       </c>
       <c r="D195">
-        <v>0.4909327123502331</v>
+        <v>0.4926743239067064</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -3156,7 +3156,7 @@
         <v>11</v>
       </c>
       <c r="D196">
-        <v>0.491948126842262</v>
+        <v>0.4936388656444617</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -3170,7 +3170,7 @@
         <v>12</v>
       </c>
       <c r="D197">
-        <v>0.4928925457197903</v>
+        <v>0.494533854295554</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -3184,7 +3184,7 @@
         <v>13</v>
       </c>
       <c r="D198">
-        <v>0.4937657038352574</v>
+        <v>0.4953591081364901</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -3198,7 +3198,7 @@
         <v>14</v>
       </c>
       <c r="D199">
-        <v>0.4945673567706772</v>
+        <v>0.496114464649517</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -3212,7 +3212,7 @@
         <v>15</v>
       </c>
       <c r="D200">
-        <v>0.4952972809160324</v>
+        <v>0.4967997805226216</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -3226,7 +3226,7 @@
         <v>16</v>
       </c>
       <c r="D201">
-        <v>0.495955273547671</v>
+        <v>0.4974149316495354</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -3240,7 +3240,7 @@
         <v>17</v>
       </c>
       <c r="D202">
-        <v>0.496541152906699</v>
+        <v>0.4979598131297277</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3254,7 +3254,7 @@
         <v>18</v>
       </c>
       <c r="D203">
-        <v>0.4970547582773781</v>
+        <v>0.4984343392684096</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -3268,7 +3268,7 @@
         <v>19</v>
       </c>
       <c r="D204">
-        <v>0.4974959500655194</v>
+        <v>0.4988384435765343</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -3282,7 +3282,7 @@
         <v>20</v>
       </c>
       <c r="D205">
-        <v>0.497864609876878</v>
+        <v>0.4991720787707949</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3296,7 +3296,7 @@
         <v>21</v>
       </c>
       <c r="D206">
-        <v>0.4981606405955515</v>
+        <v>0.4994352167736264</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -3310,7 +3310,7 @@
         <v>22</v>
       </c>
       <c r="D207">
-        <v>0.4983839664623708</v>
+        <v>0.4996278487132046</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -3324,7 +3324,7 @@
         <v>23</v>
       </c>
       <c r="D208">
-        <v>0.4985345331532985</v>
+        <v>0.4997499849234461</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -3338,7 +3338,7 @@
         <v>24</v>
       </c>
       <c r="D209">
-        <v>0.4986123078578223</v>
+        <v>0.4998016549440094</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -3352,7 +3352,7 @@
         <v>25</v>
       </c>
       <c r="D210">
-        <v>0.4986172793573529</v>
+        <v>0.4997829075202935</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -3366,7 +3366,7 @@
         <v>26</v>
       </c>
       <c r="D211">
-        <v>0.4985494581036151</v>
+        <v>0.4996938106034373</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -3380,7 +3380,7 @@
         <v>27</v>
       </c>
       <c r="D212">
-        <v>0.4984088762970463</v>
+        <v>0.4995344513503248</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -3394,7 +3394,7 @@
         <v>28</v>
       </c>
       <c r="D213">
-        <v>0.4981955879651902</v>
+        <v>0.4993049361235772</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -3408,7 +3408,7 @@
         <v>29</v>
       </c>
       <c r="D214">
-        <v>0.4979096690410922</v>
+        <v>0.4990053904915571</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -3422,7 +3422,7 @@
         <v>30</v>
       </c>
       <c r="D215">
-        <v>0.4975512174416967</v>
+        <v>0.4986359592283703</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -3436,7 +3436,7 @@
         <v>31</v>
       </c>
       <c r="D216">
-        <v>0.4971203531462376</v>
+        <v>0.4981968063138613</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -3450,7 +3450,7 @@
         <v>32</v>
       </c>
       <c r="D217">
-        <v>0.496617218274637</v>
+        <v>0.4976881149336174</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -3464,7 +3464,7 @@
         <v>33</v>
       </c>
       <c r="D218">
-        <v>0.4960419771659013</v>
+        <v>0.4971100874789667</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -3478,7 +3478,7 @@
         <v>34</v>
       </c>
       <c r="D219">
-        <v>0.4953948164565138</v>
+        <v>0.496462945546979</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -3492,7 +3492,7 @@
         <v>35</v>
       </c>
       <c r="D220">
-        <v>0.4946759451588315</v>
+        <v>0.4957469299404624</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -3506,7 +3506,7 @@
         <v>36</v>
       </c>
       <c r="D221">
-        <v>0.4938855947394787</v>
+        <v>0.4949623006679697</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -3520,7 +3520,7 @@
         <v>37</v>
       </c>
       <c r="D222">
-        <v>0.4930240191977436</v>
+        <v>0.4941093369437924</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -3534,7 +3534,7 @@
         <v>38</v>
       </c>
       <c r="D223">
-        <v>0.4920914951439731</v>
+        <v>0.4931883371879645</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -3548,7 +3548,7 @@
         <v>39</v>
       </c>
       <c r="D224">
-        <v>0.4910883218779701</v>
+        <v>0.4921996190262591</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -3562,7 +3562,7 @@
         <v>40</v>
       </c>
       <c r="D225">
-        <v>0.4900148214673844</v>
+        <v>0.4911435192901931</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -3576,7 +3576,7 @@
         <v>41</v>
       </c>
       <c r="D226">
-        <v>0.4888713388261102</v>
+        <v>0.4900203940170225</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -3590,7 +3590,7 @@
         <v>42</v>
       </c>
       <c r="D227">
-        <v>0.4876582417926818</v>
+        <v>0.4888306184497449</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -3604,7 +3604,7 @@
         <v>43</v>
       </c>
       <c r="D228">
-        <v>0.4863759212086693</v>
+        <v>0.4875745870370989</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -3618,7 +3618,7 @@
         <v>44</v>
       </c>
       <c r="D229">
-        <v>0.4850247909970716</v>
+        <v>0.4862527134335662</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -3632,7 +3632,7 @@
         <v>45</v>
       </c>
       <c r="D230">
-        <v>0.4836052882407134</v>
+        <v>0.484865430499366</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -3646,7 +3646,7 @@
         <v>46</v>
       </c>
       <c r="D231">
-        <v>0.4821178732606395</v>
+        <v>0.4834131903004612</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -3660,7 +3660,7 @@
         <v>47</v>
       </c>
       <c r="D232">
-        <v>0.4805630296945098</v>
+        <v>0.4818964641085541</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -3674,7 +3674,7 @@
         <v>48</v>
       </c>
       <c r="D233">
-        <v>0.4789412645749975</v>
+        <v>0.4803157424010899</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -3688,7 +3688,7 @@
         <v>49</v>
       </c>
       <c r="D234">
-        <v>0.4772531084081779</v>
+        <v>0.4786715348612532</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -3702,7 +3702,7 @@
         <v>50</v>
       </c>
       <c r="D235">
-        <v>0.4754991152519312</v>
+        <v>0.4769643703779716</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -3716,7 +3716,7 @@
         <v>51</v>
       </c>
       <c r="D236">
-        <v>0.4736798627943322</v>
+        <v>0.4751947970459111</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -3730,7 +3730,7 @@
         <v>52</v>
       </c>
       <c r="D237">
-        <v>0.4717959524320484</v>
+        <v>0.4733633821654825</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -3744,7 +3744,7 @@
         <v>53</v>
       </c>
       <c r="D238">
-        <v>0.4698480093487327</v>
+        <v>0.4714707122428343</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -3758,7 +3758,7 @@
         <v>54</v>
       </c>
       <c r="D239">
-        <v>0.4678366825934221</v>
+        <v>0.4695173929898573</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -3772,7 +3772,7 @@
         <v>55</v>
       </c>
       <c r="D240">
-        <v>0.4657626451589298</v>
+        <v>0.4675040493241835</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -3786,7 +3786,7 @@
         <v>56</v>
       </c>
       <c r="D241">
-        <v>0.4636265940602403</v>
+        <v>0.4654313253691861</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -3800,7 +3800,7 @@
         <v>57</v>
       </c>
       <c r="D242">
-        <v>0.4614292504129086</v>
+        <v>0.4632998844539795</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -3814,7 +3814,7 @@
         <v>58</v>
       </c>
       <c r="D243">
-        <v>0.4591713595114491</v>
+        <v>0.4611104091134177</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -3828,7 +3828,7 @@
         <v>59</v>
       </c>
       <c r="D244">
-        <v>0.4568536909077388</v>
+        <v>0.4588636010880988</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -3842,7 +3842,7 @@
         <v>60</v>
       </c>
       <c r="D245">
-        <v>0.454477038489404</v>
+        <v>0.4565601813243589</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -3856,7 +3856,7 @@
         <v>61</v>
       </c>
       <c r="D246">
-        <v>0.4520422205582205</v>
+        <v>0.4542008899742775</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -3870,7 +3870,7 @@
         <v>62</v>
       </c>
       <c r="D247">
-        <v>0.4495500799085116</v>
+        <v>0.4517864863956732</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -3884,7 +3884,7 @@
         <v>63</v>
       </c>
       <c r="D248">
-        <v>0.4470014839055344</v>
+        <v>0.4493177491521082</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -3898,7 +3898,7 @@
         <v>64</v>
       </c>
       <c r="D249">
-        <v>0.4443973245638818</v>
+        <v>0.4467954760128833</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -3912,7 +3912,7 @@
         <v>65</v>
       </c>
       <c r="D250">
-        <v>0.4417385186258761</v>
+        <v>0.4442204839530406</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -3926,7 +3926,7 @@
         <v>66</v>
       </c>
       <c r="D251">
-        <v>0.4390260076399676</v>
+        <v>0.4415936091533654</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -3940,7 +3940,7 @@
         <v>67</v>
       </c>
       <c r="D252">
-        <v>0.4362607580391213</v>
+        <v>0.4389157070003828</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -3954,7 +3954,7 @@
         <v>68</v>
       </c>
       <c r="D253">
-        <v>0.433443761219219</v>
+        <v>0.4361876520863572</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -3968,7 +3968,7 @@
         <v>69</v>
       </c>
       <c r="D254">
-        <v>0.430576033617454</v>
+        <v>0.4334103382092983</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -3982,7 +3982,7 @@
         <v>70</v>
       </c>
       <c r="D255">
-        <v>0.4276586167907245</v>
+        <v>0.4305846783729537</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -3996,7 +3996,7 @@
         <v>71</v>
       </c>
       <c r="D256">
-        <v>0.4246925774940275</v>
+        <v>0.4277116047868123</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -4010,7 +4010,7 @@
         <v>72</v>
       </c>
       <c r="D257">
-        <v>0.4216790077588587</v>
+        <v>0.4247920688661054</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -4024,7 +4024,7 @@
         <v>73</v>
       </c>
       <c r="D258">
-        <v>0.4186190249716022</v>
+        <v>0.4218270412318042</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -4038,7 +4038,7 @@
         <v>74</v>
       </c>
       <c r="D259">
-        <v>0.4155137719519317</v>
+        <v>0.4188175117106211</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -4052,7 +4052,7 @@
         <v>75</v>
       </c>
       <c r="D260">
-        <v>0.4123644170311975</v>
+        <v>0.41576448933501</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -4066,7 +4066,7 @@
         <v>76</v>
       </c>
       <c r="D261">
-        <v>0.4091721541308315</v>
+        <v>0.412669002343167</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -4080,7 +4080,7 @@
         <v>77</v>
       </c>
       <c r="D262">
-        <v>0.4059382028407347</v>
+        <v>0.4095320981790261</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -4094,7 +4094,7 @@
         <v>78</v>
       </c>
       <c r="D263">
-        <v>0.4026638084976746</v>
+        <v>0.4063548434922657</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -4108,7 +4108,7 @@
         <v>79</v>
       </c>
       <c r="D264">
-        <v>0.3993502422636848</v>
+        <v>0.4031383241383054</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -4122,7 +4122,7 @@
         <v>80</v>
       </c>
       <c r="D265">
-        <v>0.3959988012044516</v>
+        <v>0.3998836451783027</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -4136,7 +4136,7 @@
         <v>81</v>
       </c>
       <c r="D266">
-        <v>0.3926108083677171</v>
+        <v>0.3965919308791577</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -4150,7 +4150,7 @@
         <v>82</v>
       </c>
       <c r="D267">
-        <v>0.389187612861669</v>
+        <v>0.3932643247135135</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -4164,7 +4164,7 @@
         <v>83</v>
       </c>
       <c r="D268">
-        <v>0.3857305899333417</v>
+        <v>0.3899019893597511</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -4178,7 +4178,7 @@
         <v>84</v>
       </c>
       <c r="D269">
-        <v>0.3822411410470047</v>
+        <v>0.3865061067019945</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -4192,7 +4192,7 @@
         <v>85</v>
       </c>
       <c r="D270">
-        <v>0.378720693962563</v>
+        <v>0.3830778778301087</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -4206,7 +4206,7 @@
         <v>86</v>
       </c>
       <c r="D271">
-        <v>0.3751707028139486</v>
+        <v>0.3796185230397012</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -4220,7 +4220,7 @@
         <v>87</v>
       </c>
       <c r="D272">
-        <v>0.3715926481875186</v>
+        <v>0.3761292818321169</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4234,7 +4234,7 @@
         <v>88</v>
       </c>
       <c r="D273">
-        <v>0.3679880372004481</v>
+        <v>0.3726114129144452</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4248,7 +4248,7 @@
         <v>89</v>
       </c>
       <c r="D274">
-        <v>0.3643584035791301</v>
+        <v>0.3690661941995148</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -4262,7 +4262,7 @@
         <v>90</v>
       </c>
       <c r="D275">
-        <v>0.3607053077375622</v>
+        <v>0.365494922805895</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -4276,7 +4276,7 @@
         <v>91</v>
       </c>
       <c r="D276">
-        <v>0.3570303368557495</v>
+        <v>0.3618989150578977</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -4290,7 +4290,7 @@
         <v>92</v>
       </c>
       <c r="D277">
-        <v>0.3533351049580973</v>
+        <v>0.3582795064855758</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -4304,7 +4304,7 @@
         <v>93</v>
       </c>
       <c r="D278">
-        <v>0.3496212529918049</v>
+        <v>0.354638051824723</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -4318,7 +4318,7 @@
         <v>94</v>
       </c>
       <c r="D279">
-        <v>0.3458904489052651</v>
+        <v>0.3509759250168732</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -4332,7 +4332,7 @@
         <v>95</v>
       </c>
       <c r="D280">
-        <v>0.3421443877264512</v>
+        <v>0.3472945192093028</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -4346,7 +4346,7 @@
         <v>96</v>
       </c>
       <c r="D281">
-        <v>0.3383847916413202</v>
+        <v>0.3435952467550287</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -4360,7 +4360,7 @@
         <v>97</v>
       </c>
       <c r="D282">
-        <v>0.3346134100722059</v>
+        <v>0.3398795392128092</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -4374,7 +4374,7 @@
         <v>98</v>
       </c>
       <c r="D283">
-        <v>0.3308320197562118</v>
+        <v>0.336148847347142</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -4388,7 +4388,7 @@
         <v>99</v>
       </c>
       <c r="D284">
-        <v>0.3270424248236097</v>
+        <v>0.3324046411282681</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -4402,7 +4402,7 @@
         <v>100</v>
       </c>
       <c r="D285">
-        <v>0.323246456876231</v>
+        <v>0.3286484097321672</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -4416,7 +4416,7 @@
         <v>101</v>
       </c>
       <c r="D286">
-        <v>0.3194459750658642</v>
+        <v>0.3248816615405638</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -4430,7 +4430,7 @@
         <v>102</v>
       </c>
       <c r="D287">
-        <v>0.3156428661726504</v>
+        <v>0.3211059241409202</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -4444,7 +4444,7 @@
         <v>103</v>
       </c>
       <c r="D288">
-        <v>0.3118390446834796</v>
+        <v>0.3173227443264413</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -4458,7 +4458,7 @@
         <v>104</v>
       </c>
       <c r="D289">
-        <v>0.3080364528703821</v>
+        <v>0.3135336880960727</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -4472,7 +4472,7 @@
         <v>105</v>
       </c>
       <c r="D290">
-        <v>0.3042370608689253</v>
+        <v>0.3097403406545018</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -4486,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="D291">
-        <v>0.3004428667566131</v>
+        <v>0.3059443064121543</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -4500,7 +4500,7 @@
         <v>107</v>
       </c>
       <c r="D292">
-        <v>0.2966558966312715</v>
+        <v>0.3021472089852011</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -4514,7 +4514,7 @@
         <v>108</v>
       </c>
       <c r="D293">
-        <v>0.292878204689459</v>
+        <v>0.2983506911955506</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -4528,7 +4528,7 @@
         <v>109</v>
       </c>
       <c r="D294">
-        <v>0.2891118733048419</v>
+        <v>0.2945564150708533</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -4542,7 +4542,7 @@
         <v>110</v>
       </c>
       <c r="D295">
-        <v>0.2853590131066085</v>
+        <v>0.2907660618445047</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -4556,7 +4556,7 @@
         <v>111</v>
       </c>
       <c r="D296">
-        <v>0.281621763057851</v>
+        <v>0.2869813319556352</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -4570,7 +4570,7 @@
         <v>112</v>
       </c>
       <c r="D297">
-        <v>0.2779022905339694</v>
+        <v>0.2832039450491193</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -4584,7 +4584,7 @@
         <v>113</v>
       </c>
       <c r="D298">
-        <v>0.2742027914010619</v>
+        <v>0.2794356399755745</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -4598,7 +4598,7 @@
         <v>114</v>
       </c>
       <c r="D299">
-        <v>0.2705254900943186</v>
+        <v>0.2756781747913553</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -4612,7 +4612,7 @@
         <v>115</v>
       </c>
       <c r="D300">
-        <v>0.2668726396964224</v>
+        <v>0.2719333267585593</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -4626,7 +4626,7 @@
         <v>116</v>
       </c>
       <c r="D301">
-        <v>0.2632465220159422</v>
+        <v>0.2682028923450274</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -4640,7 +4640,7 @@
         <v>117</v>
       </c>
       <c r="D302">
-        <v>0.2596494476657221</v>
+        <v>0.2644886872243373</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -4654,7 +4654,7 @@
         <v>118</v>
       </c>
       <c r="D303">
-        <v>0.256083756141287</v>
+        <v>0.2607925462758098</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -4668,7 +4668,7 @@
         <v>119</v>
       </c>
       <c r="D304">
-        <v>0.2525518158992296</v>
+        <v>0.2571163235845092</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -4682,7 +4682,7 @@
         <v>120</v>
       </c>
       <c r="D305">
-        <v>0.2490560244356078</v>
+        <v>0.2534618924412337</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -4696,7 +4696,7 @@
         <v>121</v>
       </c>
       <c r="D306">
-        <v>0.2455988083643433</v>
+        <v>0.2498311453425325</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -4710,7 +4710,7 @@
         <v>122</v>
       </c>
       <c r="D307">
-        <v>0.2421826234956145</v>
+        <v>0.2462259939906912</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -4724,7 +4724,7 @@
         <v>123</v>
       </c>
       <c r="D308">
-        <v>0.2388099549142428</v>
+        <v>0.2426483692937332</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -4738,7 +4738,7 @@
         <v>124</v>
       </c>
       <c r="D309">
-        <v>0.2354833170581069</v>
+        <v>0.2391002213654264</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -4752,7 +4752,7 @@
         <v>125</v>
       </c>
       <c r="D310">
-        <v>0.2322052537965256</v>
+        <v>0.2355835195252794</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -4766,7 +4766,7 @@
         <v>126</v>
       </c>
       <c r="D311">
-        <v>0.2289783385086461</v>
+        <v>0.2321002522985441</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -4780,7 +4780,7 @@
         <v>127</v>
       </c>
       <c r="D312">
-        <v>0.2258051741618593</v>
+        <v>0.2286524274162084</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -4794,7 +4794,7 @@
         <v>128</v>
       </c>
       <c r="D313">
-        <v>0.2226883933901742</v>
+        <v>0.2252420718150077</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -4808,7 +4808,7 @@
         <v>129</v>
       </c>
       <c r="D314">
-        <v>0.2196306585726304</v>
+        <v>0.2218712316374088</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -4822,7 +4822,7 @@
         <v>130</v>
       </c>
       <c r="D315">
-        <v>0.2166346619116793</v>
+        <v>0.2185419722316318</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -4836,7 +4836,7 @@
         <v>131</v>
       </c>
       <c r="D316">
-        <v>0.2137031255115872</v>
+        <v>0.2152563781516286</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -4850,7 +4850,7 @@
         <v>132</v>
       </c>
       <c r="D317">
-        <v>0.2108388014568297</v>
+        <v>0.2120165531570986</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -4864,7 +4864,7 @@
         <v>133</v>
       </c>
       <c r="D318">
-        <v>0.2080444718904876</v>
+        <v>0.2088246202134734</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -4878,7 +4878,7 @@
         <v>134</v>
       </c>
       <c r="D319">
-        <v>0.2053229490926345</v>
+        <v>0.2056827214919393</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -4892,7 +4892,7 @@
         <v>135</v>
       </c>
       <c r="D320">
-        <v>0.2026770755587458</v>
+        <v>0.2025930183694085</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -4906,7 +4906,7 @@
         <v>136</v>
       </c>
       <c r="D321">
-        <v>0.2001097240780758</v>
+        <v>0.1995576914285463</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -4920,7 +4920,7 @@
         <v>137</v>
       </c>
       <c r="D322">
-        <v>0.1976237978120767</v>
+        <v>0.1965789404577519</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -4934,7 +4934,7 @@
         <v>138</v>
       </c>
       <c r="D323">
-        <v>0.1952222303727678</v>
+        <v>0.1936589844511712</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -4948,7 +4948,7 @@
         <v>139</v>
       </c>
       <c r="D324">
-        <v>0.1929079859011498</v>
+        <v>0.1908000616086845</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -4962,7 +4962,7 @@
         <v>140</v>
       </c>
       <c r="D325">
-        <v>0.1906840591455922</v>
+        <v>0.1880044293359177</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -4976,7 +4976,7 @@
         <v>141</v>
       </c>
       <c r="D326">
-        <v>0.1885534755402282</v>
+        <v>0.1852743642442369</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -4990,7 +4990,7 @@
         <v>142</v>
       </c>
       <c r="D327">
-        <v>0.1865192912833519</v>
+        <v>0.1826121621507483</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -5004,7 +5004,7 @@
         <v>143</v>
       </c>
       <c r="D328">
-        <v>0.1845845934158153</v>
+        <v>0.1800201380783069</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -5018,7 +5018,7 @@
         <v>144</v>
       </c>
       <c r="D329">
-        <v>0.1827524998994177</v>
+        <v>0.177500626255493</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -5032,7 +5032,7 @@
         <v>145</v>
       </c>
       <c r="D330">
-        <v>0.1810261596953061</v>
+        <v>0.17505598011664</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -5046,7 +5046,7 @@
         <v>146</v>
       </c>
       <c r="D331">
-        <v>0.1794087528423692</v>
+        <v>0.1726885723018222</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -5060,7 +5060,7 @@
         <v>147</v>
       </c>
       <c r="D332">
-        <v>0.177903490535636</v>
+        <v>0.1704007946568529</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -5074,7 +5074,7 @@
         <v>148</v>
       </c>
       <c r="D333">
-        <v>0.1765136152046529</v>
+        <v>0.1681950582332791</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -5088,7 +5088,7 @@
         <v>149</v>
       </c>
       <c r="D334">
-        <v>0.1752424005919138</v>
+        <v>0.1660737932884024</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -5102,7 +5102,7 @@
         <v>150</v>
       </c>
       <c r="D335">
-        <v>0.174093151831216</v>
+        <v>0.1640394492852554</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -5116,7 +5116,7 @@
         <v>151</v>
       </c>
       <c r="D336">
-        <v>0.1730692055260867</v>
+        <v>0.1620944948926179</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -5130,7 +5130,7 @@
         <v>152</v>
       </c>
       <c r="D337">
-        <v>0.1721739298281594</v>
+        <v>0.1602414179850053</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -5144,7 +5144,7 @@
         <v>153</v>
       </c>
       <c r="D338">
-        <v>0.1714107245155761</v>
+        <v>0.1584827256426762</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -5158,7 +5158,7 @@
         <v>154</v>
       </c>
       <c r="D339">
-        <v>0.1707830210713817</v>
+        <v>0.156820944151632</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -5172,7 +5172,7 @@
         <v>155</v>
       </c>
       <c r="D340">
-        <v>0.1702942827619222</v>
+        <v>0.1552586190036166</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -5186,7 +5186,7 @@
         <v>156</v>
       </c>
       <c r="D341">
-        <v>0.1699480047152303</v>
+        <v>0.1537983148961095</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -5200,7 +5200,7 @@
         <v>157</v>
       </c>
       <c r="D342">
-        <v>0.1697477139994364</v>
+        <v>0.1524426157323374</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -5214,7 +5214,7 @@
         <v>158</v>
       </c>
       <c r="D343">
-        <v>0.1696969697011465</v>
+        <v>0.1511941246212589</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -5228,7 +5228,7 @@
         <v>159</v>
       </c>
       <c r="D344">
-        <v>0.1697993630038491</v>
+        <v>0.1500554638775859</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -5242,7 +5242,7 @@
         <v>160</v>
       </c>
       <c r="D345">
-        <v>0.170058517266307</v>
+        <v>0.1490292750217617</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -5256,7 +5256,7 @@
         <v>161</v>
       </c>
       <c r="D346">
-        <v>0.1704780881009509</v>
+        <v>0.1481182187799783</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -5270,7 +5270,7 @@
         <v>162</v>
       </c>
       <c r="D347">
-        <v>0.1710617634522764</v>
+        <v>0.1473249750841614</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -5284,7 +5284,7 @@
         <v>163</v>
       </c>
       <c r="D348">
-        <v>0.1718132636752392</v>
+        <v>0.1466522430719805</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -5298,7 +5298,7 @@
         <v>164</v>
       </c>
       <c r="D349">
-        <v>0.1727363416136551</v>
+        <v>0.1461027410868512</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -5312,7 +5312,7 @@
         <v>165</v>
       </c>
       <c r="D350">
-        <v>0.1738347826785754</v>
+        <v>0.1456792066779215</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -5326,7 +5326,7 @@
         <v>166</v>
       </c>
       <c r="D351">
-        <v>0.1751124049267123</v>
+        <v>0.1453843966000855</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -5340,7 +5340,7 @@
         <v>167</v>
       </c>
       <c r="D352">
-        <v>0.1765730591388149</v>
+        <v>0.1452210868139772</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -5354,7 +5354,7 @@
         <v>168</v>
       </c>
       <c r="D353">
-        <v>0.1782206288980628</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -5368,7 +5368,7 @@
         <v>169</v>
       </c>
       <c r="D354">
-        <v>0.1800590306684687</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -5382,7 +5382,7 @@
         <v>170</v>
       </c>
       <c r="D355">
-        <v>0.1820922138732711</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -5396,7 +5396,7 @@
         <v>171</v>
       </c>
       <c r="D356">
-        <v>0.1843241609733382</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -5410,7 +5410,7 @@
         <v>172</v>
       </c>
       <c r="D357">
-        <v>0.1867588875455408</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -5424,7 +5424,7 @@
         <v>173</v>
       </c>
       <c r="D358">
-        <v>0.1894004423611712</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -5438,7 +5438,7 @@
         <v>174</v>
       </c>
       <c r="D359">
-        <v>0.1922529074643251</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -5452,7 +5452,7 @@
         <v>175</v>
       </c>
       <c r="D360">
-        <v>0.1953203982503058</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -5466,7 +5466,7 @@
         <v>176</v>
       </c>
       <c r="D361">
-        <v>0.1986070635440036</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -5480,7 +5480,7 @@
         <v>177</v>
       </c>
       <c r="D362">
-        <v>0.2021170856783119</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -5494,7 +5494,7 @@
         <v>178</v>
       </c>
       <c r="D363">
-        <v>0.2058546805725046</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -5508,7 +5508,7 @@
         <v>179</v>
       </c>
       <c r="D364">
-        <v>0.2098240978106457</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -5522,7 +5522,7 @@
         <v>180</v>
       </c>
       <c r="D365">
-        <v>0.2140296207199684</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -5536,7 +5536,21 @@
         <v>181</v>
       </c>
       <c r="D366">
-        <v>0.2184755664492894</v>
+        <v>0.1451920724859765</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4">
+      <c r="A367" s="2">
+        <v>43282</v>
+      </c>
+      <c r="B367">
+        <v>366</v>
+      </c>
+      <c r="C367">
+        <v>182</v>
+      </c>
+      <c r="D367">
+        <v>0.1451920724859765</v>
       </c>
     </row>
   </sheetData>
@@ -5577,7 +5591,7 @@
         <v>26</v>
       </c>
       <c r="D2">
-        <v>0.3093144257170571</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5591,7 +5605,7 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <v>0.2448254581198633</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5605,7 +5619,7 @@
         <v>28</v>
       </c>
       <c r="D4">
-        <v>0.1924845941441571</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5619,7 +5633,7 @@
         <v>29</v>
       </c>
       <c r="D5">
-        <v>0.1513570470452696</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5633,7 +5647,7 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>0.1205242973980787</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5647,7 +5661,7 @@
         <v>31</v>
       </c>
       <c r="D7">
-        <v>0.09908541068526541</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5661,7 +5675,7 @@
         <v>32</v>
       </c>
       <c r="D8">
-        <v>0.08615835488557234</v>
+        <v>0.07675116001046194</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5675,7 +5689,7 @@
         <v>33</v>
       </c>
       <c r="D9">
-        <v>0.08088131806206096</v>
+        <v>0.0767627705429038</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5689,7 +5703,7 @@
         <v>34</v>
       </c>
       <c r="D10">
-        <v>0.08241402595036908</v>
+        <v>0.07881749064042913</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5703,7 +5717,7 @@
         <v>35</v>
       </c>
       <c r="D11">
-        <v>0.08993905954696858</v>
+        <v>0.08674339072040579</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5717,7 +5731,7 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <v>0.102663172697423</v>
+        <v>0.1001761731216417</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5731,7 +5745,7 @@
         <v>37</v>
       </c>
       <c r="D13">
-        <v>0.119818609684645</v>
+        <v>0.1182300605362588</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5745,7 +5759,7 @@
         <v>38</v>
       </c>
       <c r="D14">
-        <v>0.1406644228171541</v>
+        <v>0.1400653886407473</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5759,7 +5773,7 @@
         <v>39</v>
       </c>
       <c r="D15">
-        <v>0.1644877900173341</v>
+        <v>0.1648886060959655</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5773,7 +5787,7 @@
         <v>40</v>
       </c>
       <c r="D16">
-        <v>0.1906053324096908</v>
+        <v>0.1919522745471395</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5787,7 +5801,7 @@
         <v>41</v>
       </c>
       <c r="D17">
-        <v>0.2183644319091093</v>
+        <v>0.2205550686238641</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5801,7 +5815,7 @@
         <v>42</v>
       </c>
       <c r="D18">
-        <v>0.2471445488091121</v>
+        <v>0.2500417759401017</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5815,7 +5829,7 @@
         <v>43</v>
       </c>
       <c r="D19">
-        <v>0.2763585393701164</v>
+        <v>0.2798032970941831</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5829,7 +5843,7 @@
         <v>44</v>
       </c>
       <c r="D20">
-        <v>0.305453973407691</v>
+        <v>0.309276645668807</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5843,7 +5857,7 @@
         <v>45</v>
       </c>
       <c r="D21">
-        <v>0.3339144518808156</v>
+        <v>0.3379449482310405</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5857,7 +5871,7 @@
         <v>46</v>
       </c>
       <c r="D22">
-        <v>0.3612609244801365</v>
+        <v>0.3653374443323187</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5871,7 +5885,7 @@
         <v>47</v>
       </c>
       <c r="D23">
-        <v>0.3870530072162252</v>
+        <v>0.3910294865084444</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5885,7 +5899,7 @@
         <v>48</v>
       </c>
       <c r="D24">
-        <v>0.4108903000078357</v>
+        <v>0.4146425402795896</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5899,7 +5913,7 @@
         <v>49</v>
       </c>
       <c r="D25">
-        <v>0.4324137042701625</v>
+        <v>0.4358441841502927</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5913,7 +5927,7 @@
         <v>50</v>
       </c>
       <c r="D26">
-        <v>0.4513067405030974</v>
+        <v>0.4543481096094623</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5927,7 +5941,7 @@
         <v>51</v>
       </c>
       <c r="D27">
-        <v>0.467296865879488</v>
+        <v>0.4699141211303731</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5941,7 +5955,7 @@
         <v>52</v>
       </c>
       <c r="D28">
-        <v>0.4801567918333943</v>
+        <v>0.4823481361706694</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5955,7 +5969,7 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>0.4897058016483468</v>
+        <v>0.4915021851723632</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5969,7 +5983,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>0.4958110680456049</v>
+        <v>0.4972744115618337</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5983,7 +5997,7 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <v>0.4983889707724127</v>
+        <v>0.4996090717498304</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5997,7 +6011,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>0.4974064141902574</v>
+        <v>0.4984965351314678</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -6011,7 +6025,7 @@
         <v>5</v>
       </c>
       <c r="D33">
-        <v>0.4928821448631279</v>
+        <v>0.4939732840862314</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -6025,7 +6039,7 @@
         <v>6</v>
       </c>
       <c r="D34">
-        <v>0.4848880691457708</v>
+        <v>0.4861219139779734</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -6039,7 +6053,7 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>0.4735505707719488</v>
+        <v>0.4750711331549143</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -6053,7 +6067,7 @@
         <v>8</v>
       </c>
       <c r="D36">
-        <v>0.4590518284426987</v>
+        <v>0.4609957629496431</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -6067,7 +6081,7 @@
         <v>9</v>
       </c>
       <c r="D37">
-        <v>0.4416311334145873</v>
+        <v>0.4441167376791158</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -6081,7 +6095,7 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>0.4215862070879708</v>
+        <v>0.4247011046446579</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -6095,7 +6109,7 @@
         <v>11</v>
       </c>
       <c r="D39">
-        <v>0.3992745185952519</v>
+        <v>0.4030620241319626</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -6109,7 +6123,7 @@
         <v>12</v>
       </c>
       <c r="D40">
-        <v>0.3751146023891364</v>
+        <v>0.3795587694110903</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -6123,7 +6137,7 @@
         <v>13</v>
       </c>
       <c r="D41">
-        <v>0.3495873758308929</v>
+        <v>0.3545967267364709</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -6137,7 +6151,7 @@
         <v>14</v>
       </c>
       <c r="D42">
-        <v>0.3232374567786075</v>
+        <v>0.3286273953469017</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -6151,7 +6165,7 @@
         <v>15</v>
       </c>
       <c r="D43">
-        <v>0.296674481175443</v>
+        <v>0.3021483874655484</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -6165,7 +6179,7 @@
         <v>16</v>
       </c>
       <c r="D44">
-        <v>0.2705744206378982</v>
+        <v>0.275703428299944</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -6179,7 +6193,7 @@
         <v>17</v>
       </c>
       <c r="D45">
-        <v>0.2456809000440618</v>
+        <v>0.2498823560419909</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -6193,7 +6207,7 @@
         <v>18</v>
       </c>
       <c r="D46">
-        <v>0.2228065151218717</v>
+        <v>0.2253211218679584</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -6207,7 +6221,7 @@
         <v>19</v>
       </c>
       <c r="D47">
-        <v>0.202834150037374</v>
+        <v>0.2027017899384842</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -6221,7 +6235,7 @@
         <v>20</v>
       </c>
       <c r="D48">
-        <v>0.1867182949829801</v>
+        <v>0.1827525373985753</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6235,7 +6249,7 @@
         <v>21</v>
       </c>
       <c r="D49">
-        <v>0.1754863637657191</v>
+        <v>0.166247654377605</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6249,7 +6263,7 @@
         <v>22</v>
       </c>
       <c r="D50">
-        <v>0.170240011395506</v>
+        <v>0.1540075439893167</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -6263,7 +6277,7 @@
         <v>23</v>
       </c>
       <c r="D51">
-        <v>0.172156451673388</v>
+        <v>0.14689872233182</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6277,7 +6291,7 @@
         <v>24</v>
       </c>
       <c r="D52">
-        <v>0.1824897747798097</v>
+        <v>0.1451962173899766</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6291,7 +6305,7 @@
         <v>25</v>
       </c>
       <c r="D53">
-        <v>0.2025722648628664</v>
+        <v>0.1451920724859765</v>
       </c>
     </row>
   </sheetData>
@@ -6332,7 +6346,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0.2151578829755977</v>
+        <v>0.07888993852532178</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6346,7 +6360,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>0.09079672629784867</v>
+        <v>0.07707572563648182</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6360,7 +6374,7 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>0.1136723627900217</v>
+        <v>0.1117189814066287</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -6374,7 +6388,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>0.2151846289345293</v>
+        <v>0.2171606827025941</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -6388,7 +6402,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>0.3390102794662601</v>
+        <v>0.342949367954492</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -6402,7 +6416,7 @@
         <v>12</v>
       </c>
       <c r="D7">
-        <v>0.4413900190814923</v>
+        <v>0.4445664655714586</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6416,7 +6430,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.493080759184855</v>
+        <v>0.4946132877134346</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6430,7 +6444,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0.4806695796056335</v>
+        <v>0.482041849653403</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6444,7 +6458,7 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>0.4106603160385101</v>
+        <v>0.4140750466184619</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6458,7 +6472,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0.3025834143232818</v>
+        <v>0.3077802468145904</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6472,7 +6486,7 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>0.2033812271406376</v>
+        <v>0.201829872164056</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -6486,7 +6500,7 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>0.1827619671752814</v>
+        <v>0.1481498461283536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>